<commit_message>
Add clone row for zalando receipt
</commit_message>
<xml_diff>
--- a/resources/template.xlsx
+++ b/resources/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jibo/Code/pisces/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61AC760-249B-ED4B-A00C-9E7B86AB2C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0577137A-9BAC-8C42-A5FA-9F80D878AE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5900" yWindow="2300" windowWidth="28240" windowHeight="17440" xr2:uid="{AB53A0BF-A8CA-CA4A-BBFF-AA8F62CCDC67}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="21">
   <si>
     <t>customer_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +109,14 @@
   </si>
   <si>
     <t>total_amount_text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jibo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -485,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C58A0684-37B1-9F44-AC71-F95BAE1D177C}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -625,6 +633,121 @@
         <v>51</v>
       </c>
     </row>
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>